<commit_message>
Implementing Excel file reader, Account creation page...
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="loginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="accountCreatonTest" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -27,57 +27,12 @@
     <t>Password</t>
   </si>
   <si>
-    <t>jcarter1.dsi</t>
-  </si>
-  <si>
-    <t>jcarter2.dsi</t>
-  </si>
-  <si>
-    <t>jcarter3.dsi</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>pass1.dsi</t>
-  </si>
-  <si>
-    <t>pass2.dsi</t>
-  </si>
-  <si>
-    <t>pass3.dsi</t>
-  </si>
-  <si>
-    <t>PasswordReset</t>
-  </si>
-  <si>
-    <t>jcarter4.dsi</t>
-  </si>
-  <si>
-    <t>jcarter5.dsi</t>
-  </si>
-  <si>
-    <t>pass4.dsi</t>
-  </si>
-  <si>
-    <t>pass5.dsi</t>
-  </si>
-  <si>
     <t>jcarter.dsi</t>
   </si>
   <si>
     <t>iftear</t>
   </si>
   <si>
-    <t>12345678</t>
-  </si>
-  <si>
-    <t>1234567</t>
-  </si>
-  <si>
-    <t>jcarter2.dsi2</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Prefix</t>
   </si>
   <si>
@@ -145,6 +100,66 @@
   </si>
   <si>
     <t>jcarter.dsi@gmail.com</t>
+  </si>
+  <si>
+    <t>STD_012116aa</t>
+  </si>
+  <si>
+    <t>STD_012116ab</t>
+  </si>
+  <si>
+    <t>STD_012116ac</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Verify Password</t>
+  </si>
+  <si>
+    <t>Secret Question</t>
+  </si>
+  <si>
+    <t>Secret Answer</t>
+  </si>
+  <si>
+    <t>TST01</t>
+  </si>
+  <si>
+    <t>TST02</t>
+  </si>
+  <si>
+    <t>TST03</t>
+  </si>
+  <si>
+    <t>STD_012216</t>
+  </si>
+  <si>
+    <t>TST01.STD_012216</t>
+  </si>
+  <si>
+    <t>TST02.STD_012216</t>
+  </si>
+  <si>
+    <t>TST03.STD_012216</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>01/01/1980</t>
   </si>
 </sst>
 </file>
@@ -219,12 +234,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -235,6 +250,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -283,7 +301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -318,7 +336,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -527,74 +545,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
+      <c r="B3" s="1">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1">
+        <v>12345678</v>
       </c>
     </row>
   </sheetData>
@@ -605,87 +614,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="3" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>12345678</v>
+      <c r="H1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H2" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H3" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H4" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -693,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -715,161 +795,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>31</v>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="5">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3">
         <v>29221</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="5">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3">
         <v>29221</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="5">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3">
         <v>29221</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Profile page enhancement
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
     <sheet name="accountCreatonTest" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="profileUpdateTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
-  <si>
-    <t>Test Case Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>UserName</t>
   </si>
@@ -27,12 +24,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>jcarter.dsi</t>
-  </si>
-  <si>
-    <t>iftear</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Prefix</t>
   </si>
   <si>
@@ -69,9 +60,6 @@
     <t>Email Address</t>
   </si>
   <si>
-    <t>UpdateProfile</t>
-  </si>
-  <si>
     <t>Prof.</t>
   </si>
   <si>
@@ -81,9 +69,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>Carter</t>
-  </si>
-  <si>
     <t>PhD</t>
   </si>
   <si>
@@ -102,15 +87,6 @@
     <t>jcarter.dsi@gmail.com</t>
   </si>
   <si>
-    <t>STD_012116aa</t>
-  </si>
-  <si>
-    <t>STD_012116ab</t>
-  </si>
-  <si>
-    <t>STD_012116ac</t>
-  </si>
-  <si>
     <t>Middle Name</t>
   </si>
   <si>
@@ -154,13 +130,46 @@
   </si>
   <si>
     <t>TST01.STD_012516</t>
+  </si>
+  <si>
+    <t>STD_012616aa</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>CANADA</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>a1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,14 +189,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,21 +223,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -295,7 +292,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +327,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,57 +549,28 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1">
-        <v>12345678</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -610,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -630,55 +598,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>37</v>
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1">
         <v>12345678</v>
@@ -687,30 +655,30 @@
         <v>12345678</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1">
         <v>12345678</v>
@@ -719,30 +687,30 @@
         <v>12345678</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1">
         <v>12345678</v>
@@ -751,10 +719,10 @@
         <v>12345678</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -765,193 +733,157 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="19.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="R1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="M2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="Q2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3">
-        <v>29221</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="3">
-        <v>29221</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="3">
-        <v>29221</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>27</v>
+      <c r="R2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="M4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="O2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Course Catalogs Page
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="74">
   <si>
     <t>UserName</t>
   </si>
@@ -105,15 +105,6 @@
     <t>Secret Answer</t>
   </si>
   <si>
-    <t>TST01</t>
-  </si>
-  <si>
-    <t>TST02</t>
-  </si>
-  <si>
-    <t>TST03</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -187,6 +178,66 @@
   </si>
   <si>
     <t>STD_020316bc</t>
+  </si>
+  <si>
+    <t>STD01</t>
+  </si>
+  <si>
+    <t>STD02</t>
+  </si>
+  <si>
+    <t>STD03</t>
+  </si>
+  <si>
+    <t>STD04</t>
+  </si>
+  <si>
+    <t>STD05</t>
+  </si>
+  <si>
+    <t>STD06</t>
+  </si>
+  <si>
+    <t>STD07</t>
+  </si>
+  <si>
+    <t>STD08</t>
+  </si>
+  <si>
+    <t>STD09</t>
+  </si>
+  <si>
+    <t>STD10</t>
+  </si>
+  <si>
+    <t>CHORME_020516aa</t>
+  </si>
+  <si>
+    <t>CHORME_020516ab</t>
+  </si>
+  <si>
+    <t>CHORME_020516ac</t>
+  </si>
+  <si>
+    <t>CHORME_020516ad</t>
+  </si>
+  <si>
+    <t>CHORME_020516ae</t>
+  </si>
+  <si>
+    <t>CHORME_020516af</t>
+  </si>
+  <si>
+    <t>CHORME_020516ag</t>
+  </si>
+  <si>
+    <t>CHORME_020516ah</t>
+  </si>
+  <si>
+    <t>CHORME_020516ai</t>
+  </si>
+  <si>
+    <t>CHORME_020516aj</t>
   </si>
 </sst>
 </file>
@@ -316,7 +367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,7 +402,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -560,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,26 +634,82 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -616,17 +723,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" style="1" customWidth="1"/>
@@ -671,22 +778,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1">
         <v>12345678</v>
@@ -695,30 +802,30 @@
         <v>12345678</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="G3" s="1">
         <v>12345678</v>
@@ -727,30 +834,30 @@
         <v>12345678</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1">
         <v>12345678</v>
@@ -759,10 +866,234 @@
         <v>12345678</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H5" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H6" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H7" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H8" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H9" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H10" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="H11" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +1106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
@@ -822,7 +1153,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>8</v>
@@ -840,10 +1171,10 @@
         <v>10</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>11</v>
@@ -866,22 +1197,22 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
@@ -899,13 +1230,13 @@
         <v>19</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>20</v>
@@ -914,10 +1245,10 @@
         <v>21</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -925,25 +1256,25 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>18</v>
@@ -958,13 +1289,13 @@
         <v>19</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>20</v>
@@ -973,10 +1304,10 @@
         <v>21</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -984,25 +1315,25 @@
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>18</v>
@@ -1017,13 +1348,13 @@
         <v>19</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>20</v>
@@ -1032,10 +1363,10 @@
         <v>21</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Catalog Count & Listings
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>UserName</t>
   </si>
@@ -189,27 +189,6 @@
     <t>STD03</t>
   </si>
   <si>
-    <t>STD04</t>
-  </si>
-  <si>
-    <t>STD05</t>
-  </si>
-  <si>
-    <t>STD06</t>
-  </si>
-  <si>
-    <t>STD07</t>
-  </si>
-  <si>
-    <t>STD08</t>
-  </si>
-  <si>
-    <t>STD09</t>
-  </si>
-  <si>
-    <t>STD10</t>
-  </si>
-  <si>
     <t>CHORME_020516aa</t>
   </si>
   <si>
@@ -217,27 +196,6 @@
   </si>
   <si>
     <t>CHORME_020516ac</t>
-  </si>
-  <si>
-    <t>CHORME_020516ad</t>
-  </si>
-  <si>
-    <t>CHORME_020516ae</t>
-  </si>
-  <si>
-    <t>CHORME_020516af</t>
-  </si>
-  <si>
-    <t>CHORME_020516ag</t>
-  </si>
-  <si>
-    <t>CHORME_020516ah</t>
-  </si>
-  <si>
-    <t>CHORME_020516ai</t>
-  </si>
-  <si>
-    <t>CHORME_020516aj</t>
   </si>
 </sst>
 </file>
@@ -367,7 +325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -611,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A5" sqref="A5:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +592,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
@@ -642,7 +600,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -650,65 +608,9 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -723,10 +625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>31</v>
@@ -793,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1">
         <v>12345678</v>
@@ -816,7 +718,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -825,7 +727,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G3" s="1">
         <v>12345678</v>
@@ -848,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
@@ -857,7 +759,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G4" s="1">
         <v>12345678</v>
@@ -869,230 +771,6 @@
         <v>29</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="H5" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="H6" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="H7" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="H8" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="H9" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="H10" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="H11" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="1" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assertion & Adding validation msg WebElemnets on Account Creation page
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" activeTab="1"/>
@@ -325,7 +325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -360,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -628,7 +628,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding error msg webelemnts on Password Change page
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" activeTab="1"/>
@@ -10,13 +10,14 @@
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
     <sheet name="accountCreatonTest" sheetId="2" r:id="rId2"/>
     <sheet name="profileUpdateTest" sheetId="3" r:id="rId3"/>
+    <sheet name="changePasswordTest" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>UserName</t>
   </si>
@@ -196,6 +197,27 @@
   </si>
   <si>
     <t>FF_020816ac</t>
+  </si>
+  <si>
+    <t>Current password</t>
+  </si>
+  <si>
+    <t>New password</t>
+  </si>
+  <si>
+    <t>Confirm password</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>FF_020916aa</t>
+  </si>
+  <si>
+    <t>FF_020916ab</t>
+  </si>
+  <si>
+    <t>FF_020916ac</t>
   </si>
 </sst>
 </file>
@@ -325,7 +347,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -360,7 +382,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,7 +594,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +640,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B3 B4" numberStoredAsText="1"/>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -628,7 +650,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,7 +708,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>31</v>
@@ -695,7 +717,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1">
         <v>12345678</v>
@@ -718,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -727,7 +749,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G3" s="1">
         <v>12345678</v>
@@ -750,7 +772,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
@@ -759,7 +781,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1">
         <v>12345678</v>
@@ -1054,4 +1076,68 @@
     <ignoredError sqref="O2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding dependency methods, Change password error msg logic
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>UserName</t>
   </si>
@@ -193,12 +193,6 @@
     <t>FF_020816aa</t>
   </si>
   <si>
-    <t>FF_020816ab</t>
-  </si>
-  <si>
-    <t>FF_020816ac</t>
-  </si>
-  <si>
     <t>Current password</t>
   </si>
   <si>
@@ -208,16 +202,16 @@
     <t>Confirm password</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>FF_020916aa</t>
-  </si>
-  <si>
-    <t>FF_020916ab</t>
-  </si>
-  <si>
-    <t>FF_020916ac</t>
+    <t>FF_021016aa</t>
+  </si>
+  <si>
+    <t>FF_021016ab</t>
+  </si>
+  <si>
+    <t>FF_021016ac</t>
+  </si>
+  <si>
+    <t>demo1234</t>
   </si>
 </sst>
 </file>
@@ -347,7 +341,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -382,7 +376,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,22 +611,6 @@
         <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -649,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>31</v>
@@ -717,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1">
         <v>12345678</v>
@@ -740,7 +718,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -749,7 +727,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1">
         <v>12345678</v>
@@ -772,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
@@ -781,7 +759,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G4" s="1">
         <v>12345678</v>
@@ -807,7 +785,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1061,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,13 +1073,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1109,15 +1087,15 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -1131,10 +1109,10 @@
         <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Test case info
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="86">
   <si>
     <t>UserName</t>
   </si>
@@ -212,6 +212,69 @@
   </si>
   <si>
     <t>demo1234</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-001</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-002</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-003</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-004</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-005</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-006</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-007</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-008</t>
+  </si>
+  <si>
+    <t>Verify update password success message with valid data on [Current password],[New password]&amp;[Confirm password]</t>
+  </si>
+  <si>
+    <t>Verify [Invalid] Current Password Validation with invalid data on [Current password] &amp; Valid data on [New password], [Confirm password]</t>
+  </si>
+  <si>
+    <t>Verify [Required] validation on Current Password field with [Blank] data on [Current password] &amp; [Valid] data on [New password], [Confirm password]</t>
+  </si>
+  <si>
+    <t>Verify [Min Length] validation on Current Password field with [Less than Min Length] data on [Current password] &amp; [Valid] data on [New password], [Confirm password]</t>
+  </si>
+  <si>
+    <t>Verify [Required] validation on New Password field with [Blank] data on [New password] &amp; [Valid] data on [Current password], [Confirm password]</t>
+  </si>
+  <si>
+    <t>Verify [Required] validation on Confirm Password field with [Blank] data on [Confirm password] &amp; [Valid] data on [Current password], [New password]</t>
+  </si>
+  <si>
+    <t>Verify [Matching] validation on Confirm Password field with [Unmatched] data on [Confirm password] &amp; [Valid] data on [Current password], [New password]</t>
+  </si>
+  <si>
+    <t>Verify [Min Length] validation on Confirm Password field with [Less than Min Length] data on [Confirm password], [New password] &amp; [Valid] data on [Current password]</t>
+  </si>
+  <si>
+    <t>Verify [Min Length] validation on New Password field with [Less than Min Length] data on [New password],[Confirm password] &amp; [Valid] data on [Current password]</t>
+  </si>
+  <si>
+    <t>QA-RESETPASS-009</t>
+  </si>
+  <si>
+    <t>Test Case</t>
   </si>
 </sst>
 </file>
@@ -243,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +325,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -275,12 +344,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,7 +411,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,7 +446,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -585,32 +655,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -618,159 +693,172 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2" numberStoredAsText="1"/>
+    <ignoredError sqref="C2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G2" s="1">
-        <v>12345678</v>
       </c>
       <c r="H2" s="1">
         <v>12345678</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="G3" s="1">
-        <v>12345678</v>
       </c>
       <c r="H3" s="1">
         <v>12345678</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G4" s="1">
-        <v>12345678</v>
       </c>
       <c r="H4" s="1">
         <v>12345678</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -782,121 +870,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="19.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>18</v>
@@ -905,57 +997,60 @@
         <v>18</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>18</v>
@@ -964,57 +1059,60 @@
         <v>18</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>18</v>
@@ -1023,27 +1121,30 @@
         <v>18</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1051,71 +1152,223 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="O2" numberStoredAsText="1"/>
+    <ignoredError sqref="P2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="153.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>64</v>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1234</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1234</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1234</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="E9" s="1">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="E10" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="F10" s="1">
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modifications on Profile page
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>UserName</t>
   </si>
@@ -157,9 +157,6 @@
     <t>STD03</t>
   </si>
   <si>
-    <t>FF_020816aa</t>
-  </si>
-  <si>
     <t>Current password</t>
   </si>
   <si>
@@ -235,15 +232,6 @@
     <t>Test Case</t>
   </si>
   <si>
-    <t>FF_021216aa</t>
-  </si>
-  <si>
-    <t>FF_021216ab</t>
-  </si>
-  <si>
-    <t>FF_021216ac</t>
-  </si>
-  <si>
     <t>TRUE</t>
   </si>
   <si>
@@ -257,6 +245,18 @@
   </si>
   <si>
     <t>ERP ID</t>
+  </si>
+  <si>
+    <t>FF_021516aa</t>
+  </si>
+  <si>
+    <t>FF_021616aa</t>
+  </si>
+  <si>
+    <t>FF_021616ab</t>
+  </si>
+  <si>
+    <t>FF_021616ac</t>
   </si>
 </sst>
 </file>
@@ -645,9 +645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -659,7 +661,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -673,31 +675,9 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -715,7 +695,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H4"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
@@ -749,7 +729,7 @@
         <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>7</v>
@@ -784,10 +764,10 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>31</v>
@@ -796,7 +776,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I2" s="1">
         <v>12345678</v>
@@ -822,10 +802,10 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>31</v>
@@ -834,7 +814,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I3" s="1">
         <v>12345678</v>
@@ -860,10 +840,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>31</v>
@@ -872,7 +852,7 @@
         <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I4" s="1">
         <v>12345678</v>
@@ -898,7 +878,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +907,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
@@ -1000,8 +980,8 @@
       <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>46</v>
+      <c r="E2" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>16</v>
@@ -1051,7 +1031,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>42</v>
@@ -1059,8 +1039,8 @@
       <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>46</v>
+      <c r="E3" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>31</v>
@@ -1135,22 +1115,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1158,10 +1138,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>32</v>
@@ -1178,13 +1158,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>32</v>
@@ -1198,10 +1178,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>32</v>
@@ -1215,10 +1195,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1">
         <v>1234</v>
@@ -1235,10 +1215,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1">
         <v>12345678</v>
@@ -1252,10 +1232,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1">
         <v>12345678</v>
@@ -1272,10 +1252,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1">
         <v>12345678</v>
@@ -1292,10 +1272,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1">
         <v>12345678</v>
@@ -1309,10 +1289,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="1">
         <v>12345678</v>

</xml_diff>

<commit_message>
Adding user name for Login Account Creation success/failure
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="100">
   <si>
     <t>UserName</t>
   </si>
@@ -247,16 +247,76 @@
     <t>ERP ID</t>
   </si>
   <si>
-    <t>FF_021516aa</t>
-  </si>
-  <si>
-    <t>FF_021616aa</t>
-  </si>
-  <si>
-    <t>FF_021616ab</t>
-  </si>
-  <si>
-    <t>FF_021616ac</t>
+    <t>CHROME_021816aa</t>
+  </si>
+  <si>
+    <t>CHROME_021816ab</t>
+  </si>
+  <si>
+    <t>CHROME_021816ac</t>
+  </si>
+  <si>
+    <t>CHROME_021816ad</t>
+  </si>
+  <si>
+    <t>CHROME_021816ae</t>
+  </si>
+  <si>
+    <t>CHROME_021816af</t>
+  </si>
+  <si>
+    <t>CHROME_021816ag</t>
+  </si>
+  <si>
+    <t>CHROME_021816ah</t>
+  </si>
+  <si>
+    <t>CHROME_021816ai</t>
+  </si>
+  <si>
+    <t>CHROME_021816aj</t>
+  </si>
+  <si>
+    <t>zCxab5972</t>
+  </si>
+  <si>
+    <t>zCxab5973</t>
+  </si>
+  <si>
+    <t>zCxab5974</t>
+  </si>
+  <si>
+    <t>zCxab5975</t>
+  </si>
+  <si>
+    <t>zCxab5976</t>
+  </si>
+  <si>
+    <t>zCxab5977</t>
+  </si>
+  <si>
+    <t>zCxab5978</t>
+  </si>
+  <si>
+    <t>STD04</t>
+  </si>
+  <si>
+    <t>STD05</t>
+  </si>
+  <si>
+    <t>STD06</t>
+  </si>
+  <si>
+    <t>STD07</t>
+  </si>
+  <si>
+    <t>STD08</t>
+  </si>
+  <si>
+    <t>STD09</t>
+  </si>
+  <si>
+    <t>STD10</t>
   </si>
 </sst>
 </file>
@@ -647,14 +707,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -675,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -692,10 +752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +763,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
@@ -764,7 +824,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>72</v>
@@ -776,7 +836,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I2" s="1">
         <v>12345678</v>
@@ -802,7 +862,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>73</v>
@@ -814,7 +874,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I3" s="1">
         <v>12345678</v>
@@ -840,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>74</v>
@@ -852,7 +912,7 @@
         <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I4" s="1">
         <v>12345678</v>
@@ -864,6 +924,272 @@
         <v>29</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J5" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J6" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J7" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J8" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J9" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J10" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="J11" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -878,7 +1204,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +1213,7 @@
     <col min="2" max="2" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="7" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" style="7" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Some enhancements for Page Load
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -247,36 +247,6 @@
     <t>ERP ID</t>
   </si>
   <si>
-    <t>CHROME_021816aa</t>
-  </si>
-  <si>
-    <t>CHROME_021816ab</t>
-  </si>
-  <si>
-    <t>CHROME_021816ac</t>
-  </si>
-  <si>
-    <t>CHROME_021816ad</t>
-  </si>
-  <si>
-    <t>CHROME_021816ae</t>
-  </si>
-  <si>
-    <t>CHROME_021816af</t>
-  </si>
-  <si>
-    <t>CHROME_021816ag</t>
-  </si>
-  <si>
-    <t>CHROME_021816ah</t>
-  </si>
-  <si>
-    <t>CHROME_021816ai</t>
-  </si>
-  <si>
-    <t>CHROME_021816aj</t>
-  </si>
-  <si>
     <t>zCxab5972</t>
   </si>
   <si>
@@ -317,6 +287,36 @@
   </si>
   <si>
     <t>STD10</t>
+  </si>
+  <si>
+    <t>CHROME_021916aa</t>
+  </si>
+  <si>
+    <t>CHROME_021916ac</t>
+  </si>
+  <si>
+    <t>CHROME_021916ad</t>
+  </si>
+  <si>
+    <t>CHROME_021916ae</t>
+  </si>
+  <si>
+    <t>CHROME_021916af</t>
+  </si>
+  <si>
+    <t>CHROME_021916ag</t>
+  </si>
+  <si>
+    <t>CHROME_021916ah</t>
+  </si>
+  <si>
+    <t>CHROME_021916ai</t>
+  </si>
+  <si>
+    <t>CHROME_021916aj</t>
+  </si>
+  <si>
+    <t>CHROME_021916ab</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +824,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>72</v>
@@ -836,7 +836,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="I2" s="1">
         <v>12345678</v>
@@ -862,7 +862,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>73</v>
@@ -874,7 +874,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="I3" s="1">
         <v>12345678</v>
@@ -900,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>74</v>
@@ -912,7 +912,7 @@
         <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="I4" s="1">
         <v>12345678</v>
@@ -932,16 +932,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>31</v>
@@ -950,7 +950,7 @@
         <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="I5" s="1">
         <v>12345678</v>
@@ -970,16 +970,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>31</v>
@@ -988,7 +988,7 @@
         <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="I6" s="1">
         <v>12345678</v>
@@ -1008,16 +1008,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>31</v>
@@ -1026,7 +1026,7 @@
         <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="I7" s="1">
         <v>12345678</v>
@@ -1046,16 +1046,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>31</v>
@@ -1064,7 +1064,7 @@
         <v>21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="I8" s="1">
         <v>12345678</v>
@@ -1084,16 +1084,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>31</v>
@@ -1102,7 +1102,7 @@
         <v>21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="I9" s="1">
         <v>12345678</v>
@@ -1122,16 +1122,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>31</v>
@@ -1140,7 +1140,7 @@
         <v>21</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="I10" s="1">
         <v>12345678</v>
@@ -1160,16 +1160,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>31</v>
@@ -1178,7 +1178,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="I11" s="1">
         <v>12345678</v>
@@ -1203,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1307,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>16</v>
@@ -1366,7 +1366,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Adding ERP ID field
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
   <si>
     <t>UserName</t>
   </si>
@@ -235,88 +235,49 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>zCxab5969</t>
-  </si>
-  <si>
-    <t>zCxab5970</t>
-  </si>
-  <si>
-    <t>zCxab5971</t>
-  </si>
-  <si>
     <t>ERP ID</t>
   </si>
   <si>
-    <t>zCxab5972</t>
-  </si>
-  <si>
-    <t>zCxab5973</t>
-  </si>
-  <si>
-    <t>zCxab5974</t>
-  </si>
-  <si>
-    <t>zCxab5975</t>
-  </si>
-  <si>
-    <t>zCxab5976</t>
-  </si>
-  <si>
-    <t>zCxab5977</t>
-  </si>
-  <si>
-    <t>zCxab5978</t>
-  </si>
-  <si>
     <t>STD04</t>
   </si>
   <si>
     <t>STD05</t>
   </si>
   <si>
+    <t>FF_022316aa</t>
+  </si>
+  <si>
+    <t>abcd1234</t>
+  </si>
+  <si>
+    <t>abcde1234</t>
+  </si>
+  <si>
+    <t>abcd12345</t>
+  </si>
+  <si>
+    <t>abcdefgh</t>
+  </si>
+  <si>
     <t>STD06</t>
   </si>
   <si>
-    <t>STD07</t>
-  </si>
-  <si>
-    <t>STD08</t>
-  </si>
-  <si>
-    <t>STD09</t>
-  </si>
-  <si>
-    <t>STD10</t>
-  </si>
-  <si>
-    <t>CHROME_021916aa</t>
-  </si>
-  <si>
-    <t>CHROME_021916ac</t>
-  </si>
-  <si>
-    <t>CHROME_021916ad</t>
-  </si>
-  <si>
-    <t>CHROME_021916ae</t>
-  </si>
-  <si>
-    <t>CHROME_021916af</t>
-  </si>
-  <si>
-    <t>CHROME_021916ag</t>
-  </si>
-  <si>
-    <t>CHROME_021916ah</t>
-  </si>
-  <si>
-    <t>CHROME_021916ai</t>
-  </si>
-  <si>
-    <t>CHROME_021916aj</t>
-  </si>
-  <si>
-    <t>CHROME_021916ab</t>
+    <t>FF_022316aae</t>
+  </si>
+  <si>
+    <t>FF_022316aaf</t>
+  </si>
+  <si>
+    <t>FF_022316aag</t>
+  </si>
+  <si>
+    <t>FF_022316aah</t>
+  </si>
+  <si>
+    <t>FF_022316aai</t>
+  </si>
+  <si>
+    <t>FF_022316aad</t>
   </si>
 </sst>
 </file>
@@ -708,7 +669,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,40 +696,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -780,16 +738,16 @@
         <v>51</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>7</v>
@@ -817,17 +775,14 @@
       <c r="A2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>31</v>
@@ -836,13 +791,13 @@
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J2" s="1">
-        <v>12345678</v>
+        <v>81</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>29</v>
@@ -856,16 +811,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>31</v>
@@ -874,13 +829,13 @@
         <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J3" s="1">
-        <v>12345678</v>
+        <v>82</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>29</v>
@@ -894,16 +849,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>31</v>
@@ -912,13 +867,13 @@
         <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J4" s="1">
-        <v>12345678</v>
+        <v>83</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>29</v>
@@ -932,16 +887,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>31</v>
@@ -950,13 +905,13 @@
         <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J5" s="1">
-        <v>12345678</v>
+        <v>84</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>29</v>
@@ -970,16 +925,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>31</v>
@@ -988,13 +943,13 @@
         <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J6" s="1">
-        <v>12345678</v>
+        <v>85</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>29</v>
@@ -1008,16 +963,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>31</v>
@@ -1026,170 +981,18 @@
         <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J7" s="1">
-        <v>12345678</v>
+        <v>86</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I8" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J8" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I9" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J9" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I10" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J10" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="J11" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1203,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1110,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>16</v>
@@ -1366,7 +1169,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
ERP ID logic implementation...
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -235,39 +235,9 @@
     <t>abcd1234</t>
   </si>
   <si>
-    <t>FF_030116aa</t>
-  </si>
-  <si>
-    <t>FF_030116ab</t>
-  </si>
-  <si>
     <t>abcd1235</t>
   </si>
   <si>
-    <t>FF_030116ac</t>
-  </si>
-  <si>
-    <t>FF_030116ad</t>
-  </si>
-  <si>
-    <t>FF_030116ae</t>
-  </si>
-  <si>
-    <t>FF_030116af</t>
-  </si>
-  <si>
-    <t>FF_030116ag</t>
-  </si>
-  <si>
-    <t>FF_030116ah</t>
-  </si>
-  <si>
-    <t>FF_030116ai</t>
-  </si>
-  <si>
-    <t>FF_030116aj</t>
-  </si>
-  <si>
     <t>01/01/1981</t>
   </si>
   <si>
@@ -341,6 +311,36 @@
   </si>
   <si>
     <t>abcd1243</t>
+  </si>
+  <si>
+    <t>FF_030316aa</t>
+  </si>
+  <si>
+    <t>FF_030316ab</t>
+  </si>
+  <si>
+    <t>FF_030316ac</t>
+  </si>
+  <si>
+    <t>FF_030316ad</t>
+  </si>
+  <si>
+    <t>FF_030316ae</t>
+  </si>
+  <si>
+    <t>FF_030316af</t>
+  </si>
+  <si>
+    <t>FF_030316ag</t>
+  </si>
+  <si>
+    <t>FF_030316ah</t>
+  </si>
+  <si>
+    <t>FF_030316ai</t>
+  </si>
+  <si>
+    <t>FF_030316aj</t>
   </si>
 </sst>
 </file>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,10 +759,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +847,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>31</v>
@@ -856,13 +856,13 @@
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>29</v>
@@ -876,7 +876,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>44</v>
@@ -885,22 +885,22 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>29</v>
@@ -914,31 +914,31 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>29</v>
@@ -952,31 +952,31 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>29</v>
@@ -990,31 +990,31 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>29</v>
@@ -1028,31 +1028,31 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>29</v>
@@ -1066,31 +1066,31 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>29</v>
@@ -1104,31 +1104,31 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>29</v>
@@ -1142,31 +1142,31 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>29</v>
@@ -1180,31 +1180,31 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>29</v>
@@ -1224,7 +1224,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1327,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Login Account creation page enhancements
</commit_message>
<xml_diff>
--- a/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
+++ b/QuickAdmitAutomation/src/test/resources/testData/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6435" tabRatio="659" firstSheet="1" activeTab="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="83">
   <si>
     <t>UserName</t>
   </si>
@@ -259,16 +259,13 @@
     <t>TST02</t>
   </si>
   <si>
-    <t>STD_040216aa</t>
-  </si>
-  <si>
     <t>Verify failure message while creating new Student Account with [duplicate data] on [First Name, Last Name] input fields</t>
   </si>
   <si>
-    <t>STD_040216ab</t>
-  </si>
-  <si>
-    <t>STD_040216bb</t>
+    <t>STD_040516aa</t>
+  </si>
+  <si>
+    <t>STD_040516ab</t>
   </si>
 </sst>
 </file>
@@ -413,7 +410,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -448,7 +445,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -703,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +786,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>31</v>
@@ -798,13 +795,13 @@
         <v>21</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>29</v>
@@ -821,7 +818,7 @@
         <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>69</v>
@@ -833,7 +830,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>31</v>
@@ -877,7 +874,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
@@ -886,13 +883,13 @@
         <v>21</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>29</v>

</xml_diff>